<commit_message>
Implement counting of user reponse.
</commit_message>
<xml_diff>
--- a/custom/chat_history.xlsx
+++ b/custom/chat_history.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -406,14 +406,14 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>14-03-27</t>
+          <t>18:01:16</t>
         </is>
       </c>
       <c r="C1" t="n">
         <v>-615761128</v>
       </c>
       <c r="D1" t="n">
-        <v>1107423707</v>
+        <v>741216406</v>
       </c>
     </row>
     <row r="2">
@@ -424,7 +424,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>14-03-35</t>
+          <t>18:01:18</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -442,13 +442,67 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>14-03-41</t>
+          <t>18:01:27</t>
         </is>
       </c>
       <c r="C3" t="n">
+        <v>-485430438</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1107423707</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2021-11-06</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>18:01:30</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>-615761128</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D4" t="n">
+        <v>741216406</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2021-11-06</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>18:01:40</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>-615761128</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1107423707</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2021-11-06</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>18:01:42</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>-485430438</v>
+      </c>
+      <c r="D6" t="n">
         <v>1107423707</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Project finish, waiting for aditional changes.
</commit_message>
<xml_diff>
--- a/custom/chat_history.xlsx
+++ b/custom/chat_history.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -390,123 +390,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>2021-11-06</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>18:01:16</t>
-        </is>
-      </c>
-      <c r="C1" t="n">
-        <v>-615761128</v>
-      </c>
-      <c r="D1" t="n">
-        <v>741216406</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2021-11-06</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>18:01:18</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>-615761128</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1107423707</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2021-11-06</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>18:01:27</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>-485430438</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1107423707</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2021-11-06</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>18:01:30</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>-615761128</v>
-      </c>
-      <c r="D4" t="n">
-        <v>741216406</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2021-11-06</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>18:01:40</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>-615761128</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1107423707</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2021-11-06</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>18:01:42</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>-485430438</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1107423707</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>